<commit_message>
Sections no longer go across pages.
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="weapons" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,8 @@
     <sheet name="chalice_accessories" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="edible_accessories" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="monsters" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="monsters_rva" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Sheet10" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
   <si>
     <t xml:space="preserve">Weapon</t>
   </si>
@@ -197,10 +199,67 @@
     <t xml:space="preserve">If the pressure roll is less than or equal to your Luck stat, don't thicken the miasma.</t>
   </si>
   <si>
-    <t xml:space="preserve">Focus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Racket</t>
+    <t xml:space="preserve">Myrrh Leaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear a Status Effect from yourself</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hearts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vulnerabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goblin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vulnerable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lightning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appears in groups of 3 to 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdf</t>
   </si>
 </sst>
 </file>
@@ -210,7 +269,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -232,6 +291,13 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +316,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,6 +340,24 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -289,13 +373,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Pivot Table Category" xfId="20"/>
+    <cellStyle name="Pivot Table Corner" xfId="21"/>
+    <cellStyle name="Pivot Table Field" xfId="22"/>
+    <cellStyle name="Pivot Table Result" xfId="23"/>
+    <cellStyle name="Pivot Table Title" xfId="24"/>
+    <cellStyle name="Pivot Table Value" xfId="25"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -309,6 +399,17 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Import1" displayName="Import1" ref="A1:D2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="4">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Type"/>
+    <tableColumn id="3" name="Description"/>
+    <tableColumn id="4" name="Monster"/>
+  </tableColumns>
+</table>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -317,7 +418,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -423,6 +524,66 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -431,7 +592,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -562,7 +723,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -718,13 +879,13 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="86.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="86.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -764,12 +925,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -813,7 +974,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -857,32 +1018,31 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.53"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -900,34 +1060,132 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.41"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.41"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TODO Lists, GM Section Start, Reorg, Malboro
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="weapons" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,8 +16,6 @@
     <sheet name="chalice_accessories" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="edible_accessories" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="monsters" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="monsters_rva" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Sheet10" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
   <si>
     <t xml:space="preserve">Weapon</t>
   </si>
@@ -193,18 +191,45 @@
     <t xml:space="preserve">Rolling a 2 also counts as a Crit.</t>
   </si>
   <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crystal Feather</t>
   </si>
   <si>
     <t xml:space="preserve">If the pressure roll is less than or equal to your Luck stat, don't thicken the miasma.</t>
   </si>
   <si>
+    <t xml:space="preserve">Piece of bark of a Myrrh tree.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Myrrh Leaf</t>
   </si>
   <si>
     <t xml:space="preserve">Clear a Status Effect from yourself</t>
   </si>
   <si>
+    <t xml:space="preserve">Leaf of a Myrrh tree, glowing with clean air.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phoenix Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you lose your last heart, this revives you at 1 heart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic flower. Looks like a flame and a feather.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strange Liquid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heal all your hearts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rare drink. Probably Myrrh dew and herbs.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Monster</t>
   </si>
   <si>
@@ -230,36 +255,6 @@
   </si>
   <si>
     <t xml:space="preserve">Goblin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vulnerable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lightning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appears in groups of 3 to 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asdf</t>
   </si>
 </sst>
 </file>
@@ -387,27 +382,7 @@
     <cellStyle name="Pivot Table Title" xfId="24"/>
     <cellStyle name="Pivot Table Value" xfId="25"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Import1" displayName="Import1" ref="A1:D2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <tableColumns count="4">
-    <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Type"/>
-    <tableColumn id="3" name="Description"/>
-    <tableColumn id="4" name="Monster"/>
-  </tableColumns>
-</table>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,7 +393,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -521,66 +496,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <tableParts>
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -925,7 +840,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -952,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -971,10 +886,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -990,13 +905,19 @@
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1015,10 +936,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1033,16 +954,42 @@
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1074,33 +1021,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>3</v>
@@ -1113,79 +1060,6 @@
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.41"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add starting accessory information
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="weapons" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
   <si>
     <t xml:space="preserve">Weapon</t>
   </si>
@@ -195,6 +195,24 @@
   </si>
   <si>
     <t xml:space="preserve">Rolling a 2 also counts as a Crit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Makeshift Shield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Extra Heart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gauntlets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lilties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plain Helmet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old Belt</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
@@ -800,7 +818,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -851,10 +869,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -881,6 +899,50 @@
         <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -920,18 +982,18 @@
         <v>18</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -969,40 +1031,40 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1035,33 +1097,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>3</v>

</xml_diff>